<commit_message>
added pilots excel file to keep track of feedback
</commit_message>
<xml_diff>
--- a/sesres.xlsx
+++ b/sesres.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb08\GitHub\fast_schema_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="282" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -427,11 +427,82 @@
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Last session with 3 new items:</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-GB"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Compare exact "correct"</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> to "rougly correct" responses.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -447,6 +518,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -462,6 +536,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -477,6 +554,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -492,6 +572,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -507,6 +590,117 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -531,7 +725,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -546,7 +752,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -561,7 +779,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -576,7 +806,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -591,7 +833,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -606,7 +860,181 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -1301,6 +1729,62 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sessions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1366,6 +1850,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Performance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2055,18 +2595,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>70758</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1828800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>2305050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>118383</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="stage"/>
@@ -2083,7 +2623,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2093,7 +2633,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7610475" y="2343150"/>
+              <a:off x="9688286" y="2737758"/>
               <a:ext cx="1828800" cy="2524125"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2127,15 +2667,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:colOff>606878</xdr:colOff>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2258786</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>109658</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6812,7 +7352,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A1:H13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField showAll="0"/>
@@ -6937,7 +7477,7 @@
     <dataField name="Average of correct" fld="3" subtotal="average" baseField="14" baseItem="0"/>
     <dataField name="Average of roughly_correct" fld="16" subtotal="average" baseField="14" baseItem="0"/>
   </dataFields>
-  <chartFormats count="38">
+  <chartFormats count="50">
     <chartFormat chart="0" format="24" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -7388,6 +7928,150 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="2" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="14" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="15" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="18" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="20" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="23" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -7709,8 +8393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q241"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:Q241"/>
+    <sheetView topLeftCell="A93" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A195" sqref="A195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19736,20 +20420,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" customWidth="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.42578125" customWidth="1"/>
     <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37.42578125" bestFit="1" customWidth="1"/>

</xml_diff>